<commit_message>
BAEL-7278 Modify the code based on the feedback
</commit_message>
<xml_diff>
--- a/pdf-2/src/main/resources/excelsample.xlsx
+++ b/pdf-2/src/main/resources/excelsample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wynnteo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wynnteo/Desktop/Github/tutorials/pdf-2/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCA2B84-3B5B-4642-A039-E2DEF8298922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61601EF-4E01-7347-813D-DE466F095BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18420" yWindow="5280" windowWidth="24840" windowHeight="18220" xr2:uid="{342A9D1D-3143-2D49-8964-805E47EFFA50}"/>
+    <workbookView xWindow="13740" yWindow="3280" windowWidth="24840" windowHeight="18220" xr2:uid="{342A9D1D-3143-2D49-8964-805E47EFFA50}"/>
   </bookViews>
   <sheets>
     <sheet name="Order List Page 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>No.</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>A100006</t>
+  </si>
+  <si>
+    <t>Paid</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -100,58 +109,51 @@
     </font>
     <font>
       <b/>
+      <sz val="14"/>
+      <color theme="2"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Courier New"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <i/>
       <sz val="12"/>
       <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Courier New"/>
+      <family val="1"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Courier New"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -163,12 +165,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -176,19 +178,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,21 +535,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B87062-8059-0A4B-A020-9C74291956BC}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" activeCellId="1" sqref="B4 G4"/>
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -530,89 +562,110 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>56.8</v>
       </c>
+      <c r="E2" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>78.900000000000006</v>
       </c>
+      <c r="E3" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" ht="24" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:5" ht="22" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="8">
         <v>108.9</v>
       </c>
+      <c r="E4" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="9">
         <v>23.5</v>
       </c>
+      <c r="E5" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>66.8</v>
       </c>
+      <c r="E6" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="5">
         <v>34.299999999999997</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>